<commit_message>
Update libcc/resources/libreg.xlsx to add rst.h anaylsis
</commit_message>
<xml_diff>
--- a/libcc/resources/libreg.xlsx
+++ b/libcc/resources/libreg.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16620" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16620" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="sim.h" sheetId="1" r:id="rId1"/>
+    <sheet name="rst.h" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="98">
   <si>
     <t>void     regSimLoadTcError      (struct reg_sim_load_pars *sim_load_pars, struct reg_load_pars *load_pars, float sim_load_tc_error);</t>
   </si>
@@ -36,15 +37,9 @@
     <t>void     regSimLoadSetVoltage   (struct reg_sim_load_pars *pars, struct reg_sim_load_vars *vars, float v_init);</t>
   </si>
   <si>
-    <t>float    regSimLoadRT           (struct reg_sim_load_pars *pars, struct reg_sim_load_vars *vars, float voltage);</t>
-  </si>
-  <si>
     <t>void     regSimVsInitTustin     (struct reg_sim_vs_pars   *pars, float iter_period, float bandwidth, float z, float tau_zero);</t>
   </si>
   <si>
-    <t>uint32_t regSimVsInit           (struct reg_sim_vs_pars   *pars, struct reg_sim_vs_vars   *vars, float v_ref_delay_iters);</t>
-  </si>
-  <si>
     <t>float    regSimVsInitHistory    (struct reg_sim_vs_pars   *pars, struct reg_sim_vs_vars   *vars, float v_ref);</t>
   </si>
   <si>
@@ -69,9 +64,6 @@
     <t xml:space="preserve">    uint32_t                    vs_undersampled_flag;           // Simulated voltage source is under-sampled flag</t>
   </si>
   <si>
-    <t xml:space="preserve">    struct reg_load_pars load_pars;                             // Simulated load parameters</t>
-  </si>
-  <si>
     <t>};</t>
   </si>
   <si>
@@ -157,16 +149,334 @@
   </si>
   <si>
     <t>Vars</t>
+  </si>
+  <si>
+    <t>vs bandwidth</t>
+  </si>
+  <si>
+    <t>vs z</t>
+  </si>
+  <si>
+    <t>vs tau_zero</t>
+  </si>
+  <si>
+    <t>void     regSimVsInit           (struct reg_sim_vs_pars   *pars, struct reg_sim_vs_vars   *vars, float v_ref_delay_iters);</t>
+  </si>
+  <si>
+    <t>float    regSimLoadRT           (struct reg_sim_load_pars *pars, struct reg_sim_load_vars *vars, uint32_t vs_undersampled_flag, float voltage);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    struct reg_load_pars        load_pars;                      // Simulated load parameters</t>
+  </si>
+  <si>
+    <t>float    regRstCalcActRT          (struct reg_rst_pars *pars, struct reg_rst_vars *vars, float ref, float meas);</t>
+  </si>
+  <si>
+    <t>float    regRstCalcRefRT          (struct reg_rst_pars *pars, struct reg_rst_vars *vars, float act, float meas);</t>
+  </si>
+  <si>
+    <t>void     regRstTrackDelayRT       (struct reg_rst_vars *vars, float period, float max_rate);</t>
+  </si>
+  <si>
+    <t>float    regRstDelayedRefRT       (struct reg_rst_pars *pars, struct reg_rst_vars *vars, uint32_t iteration_index);</t>
+  </si>
+  <si>
+    <t>float    regRstAverageVrefRT      (struct reg_rst_vars *vars);</t>
+  </si>
+  <si>
+    <t>struct reg_rst                                                  // RST polynomial arrays and track delay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    double                      r[REG_N_RST_COEFFS];            // R polynomial coefficients (meas)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    double                      s[REG_N_RST_COEFFS];            // S polynomial coefficients (act)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    double                      t[REG_N_RST_COEFFS];            // T polynomial coefficients (ref)</t>
+  </si>
+  <si>
+    <t>struct reg_rst_pars                                             // RST algorithm parameters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    enum reg_status             status;                         // Regulation parameters status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    enum reg_mode               reg_mode;                       // Regulation mode (REG_CURRENT | REG_FIELD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    uint32_t                    period_iters;                   // Regulation period (in iterations)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    uint32_t                    alg_index;                      // Algorithm index (1-5) - based on pure delay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    uint32_t                    dead_beat;                      // 0 = not dead-beat, 1-3 = dead-beat(1-3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    double                      period;                         // Regulation period</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       inv_period_iters;               // 1/period_iters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       ref_advance;                    // Reference advance time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       pure_delay_periods;             // Pure delay in regulation periods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       track_delay_periods;            // Track delay in regulation periods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       ref_delay_periods;              // Ref delay in regulation periods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    double                      inv_s0;                         // Store 1/S[0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    double                      t0_correction;                  // Correction to t[0] for rounding errors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    double                      inv_corrected_t0;               // Store 1/(T[0]+ t0_correction)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    struct reg_rst              rst;                            // RST polynomials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    double                      a   [REG_N_RST_COEFFS];         // Plant numerator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    double                      b   [REG_N_RST_COEFFS];         // Plant denominator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    double                      as  [REG_N_RST_COEFFS];         // A.S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    double                      asbr[REG_N_RST_COEFFS];         // A.S + B.R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    int32_t                     jurys_result;                   // Jury's test result index (0=OK)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       min_auxpole_hz;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       modulus_margin;                 // Modulus margin = min(abs_S_p_y)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       modulus_margin_freq;            // Frequency for Modulus margin</t>
+  </si>
+  <si>
+    <t>struct reg_rst_vars                                             // RST algorithm variables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    uint32_t                    history_index;                  // Index to latest entry in the history</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       prev_ref_rate;                  // Ref rate from previous iteration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       meas_track_delay_periods;       // Measured track_delay in regulation periods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       ref [REG_RST_HISTORY_MASK+1];   // RST calculated reference history</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       meas[REG_RST_HISTORY_MASK+1];   // RST measurement history</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       act [REG_RST_HISTORY_MASK+1];   // RST actuation history</t>
+  </si>
+  <si>
+    <t>Internal</t>
+  </si>
+  <si>
+    <t>period_iters</t>
+  </si>
+  <si>
+    <t>auxpol1_hz</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">enum reg_status regRstInit        (struct reg_rst_pars *pars, double iter_period, uint32_t </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>period_iters</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                   struct reg_load_pars </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>*load,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t xml:space="preserve"> float </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>auxpole1_hz,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t xml:space="preserve"> float </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>auxpoles2_hz,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t xml:space="preserve"> float </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>auxpoles2_z,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                   float </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>auxpole4_hz,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t xml:space="preserve"> float </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>auxpole5_hz,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                   float </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>pure_delay_periods,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t xml:space="preserve"> float </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>track_delay_periods,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t xml:space="preserve"> enum reg_mode reg_mode,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                   struct reg_rst </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>*manual);</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -183,13 +493,39 @@
       <color theme="1"/>
       <name val="Consolas"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Consolas"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -221,27 +557,51 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Input" xfId="1" builtinId="20"/>
+  <cellStyles count="11">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -571,10 +931,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E49"/>
+  <dimension ref="B2:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -586,271 +946,627 @@
     <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5">
+    <row r="2" spans="2:6">
       <c r="C2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>38</v>
-      </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="2:5">
+    <row r="3" spans="2:6">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5">
+    </row>
+    <row r="4" spans="2:6">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="C14" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="2:5">
-      <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5">
-      <c r="B9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5">
-      <c r="B10" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5">
-      <c r="B11" s="1" t="s">
+    <row r="15" spans="2:6">
+      <c r="B15" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="2:5">
-      <c r="B12" s="1" t="s">
+      <c r="C15" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="B16" s="1" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5">
-      <c r="C14" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5">
-      <c r="B15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5">
-      <c r="B16" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="17" spans="2:4">
       <c r="B17" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="B18" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4">
-      <c r="B22" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="2:4">
       <c r="B25" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="2:4">
       <c r="B26" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="2:4">
       <c r="B27" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="2:4">
       <c r="B29" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="2:4">
       <c r="B30" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="2:4">
       <c r="B31" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4">
-      <c r="B32" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="2:4">
       <c r="B33" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4">
+      <c r="B34" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="2:4">
       <c r="B35" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
     </row>
     <row r="36" spans="2:4">
       <c r="B36" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37" spans="2:4">
       <c r="B37" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="38" spans="2:4">
       <c r="B38" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="39" spans="2:4">
       <c r="B39" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40" spans="2:4">
       <c r="B40" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="41" spans="2:4">
       <c r="B41" s="1" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
     </row>
     <row r="42" spans="2:4">
       <c r="B42" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4">
-      <c r="B43" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4">
+      <c r="B44" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="2:4">
       <c r="B45" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46" spans="2:4">
       <c r="B46" s="1" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
     </row>
     <row r="47" spans="2:4">
       <c r="B47" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="48" spans="2:4">
       <c r="B48" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2">
-      <c r="B49" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="3.6640625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="133.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7">
+      <c r="C2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="2:7">
+      <c r="B3" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7">
+      <c r="B11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7">
+      <c r="B12" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7">
+      <c r="C14" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7">
+      <c r="B15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7">
+      <c r="B16" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3">
+      <c r="B20" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3">
+      <c r="B23" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3">
+      <c r="B24" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3">
+      <c r="B25" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3">
+      <c r="B26" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3">
+      <c r="B27" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3">
+      <c r="B28" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3">
+      <c r="B29" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3">
+      <c r="B30" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3">
+      <c r="B31" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3">
+      <c r="B32" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2">
+      <c r="B38" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2">
+      <c r="B39" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2">
+      <c r="B41" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2">
+      <c r="B42" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2">
+      <c r="B43" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2">
+      <c r="B44" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2">
+      <c r="B45" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2">
+      <c r="B46" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2">
+      <c r="B47" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4">
+      <c r="B49" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4">
+      <c r="B50" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4">
+      <c r="B51" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4">
+      <c r="B52" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4">
+      <c r="B53" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4">
+      <c r="B54" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4">
+      <c r="B55" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4">
+      <c r="B56" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4">
+      <c r="B57" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update libcc/resources/libreg.xlsx to and analysis of meas.h, load.h and lim.h
</commit_message>
<xml_diff>
--- a/libcc/resources/libreg.xlsx
+++ b/libcc/resources/libreg.xlsx
@@ -4,11 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16620" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16620" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="sim.h" sheetId="1" r:id="rId1"/>
-    <sheet name="rst.h" sheetId="2" r:id="rId2"/>
+    <sheet name="lim.h" sheetId="6" r:id="rId1"/>
+    <sheet name="load.h" sheetId="5" r:id="rId2"/>
+    <sheet name="meas.h" sheetId="4" r:id="rId3"/>
+    <sheet name="rst.h" sheetId="2" r:id="rId4"/>
+    <sheet name="sim.h" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="215">
   <si>
     <t>void     regSimLoadTcError      (struct reg_sim_load_pars *sim_load_pars, struct reg_load_pars *load_pars, float sim_load_tc_error);</t>
   </si>
@@ -459,6 +462,815 @@
         <rFont val="Consolas"/>
       </rPr>
       <t>*manual);</t>
+    </r>
+  </si>
+  <si>
+    <t>void     regMeasFilterRT           (struct reg_meas_filter *filter);</t>
+  </si>
+  <si>
+    <t>void     regMeasFilterInitBuffer   (struct reg_meas_filter *filter, int32_t *buf);</t>
+  </si>
+  <si>
+    <t>void     regMeasSetRegSelect       (struct reg_meas_filter *filter, enum reg_meas_select reg_select);</t>
+  </si>
+  <si>
+    <t>float    regMeasNoiseAndToneRT     (struct reg_noise_and_tone *noise_and_tone);</t>
+  </si>
+  <si>
+    <t>void     regMeasRateRT             (struct reg_meas_rate *meas_rate, float filtered_meas, float period, int32_t period_iters);</t>
+  </si>
+  <si>
+    <t>struct reg_meas_signal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                 signal;                                 // Measurement signal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    enum reg_meas_status  status;                                 // Measurement signal status</t>
+  </si>
+  <si>
+    <t>struct reg_meas_filter                                            // Measurement filter parameters and variables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    uint32_t              enable;                                 // Enable filter control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    uint32_t              extrapolation_len_iters;                // Extrapolation length (normally regulation period)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    uint32_t              extrapolation_index;                    // Index to oldest sample in extrapolation buffer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    uint32_t              fir_length[2];                          // FIR filter length for two cascaded stages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    uint32_t              fir_index[2];                           // Index to oldest sample in FIR buffers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    int32_t               fir_accumulator[2];                     // FIR filter accumulator for two cascaded stages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    int32_t              *fir_buf[2];                             // Pointers to buffers for two cascaded FIR stages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                *extrapolation_buf;                      // Pointer to buffer for extrapolation stage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                 max_meas_value;                         // Maximum value that can be filtered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                 float_to_integer;                       // Factor to convert unfiltered measurement to integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                 integer_to_float;                       // Factor to converter integer to filtered measurement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                 extrapolation_factor;                   // Extrapolation factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    enum reg_meas_select  reg_select;                             // Regulation measurement selector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                 delay_iters[REG_MEAS_NUM_SIGNALS];      // Delay for each signal in iterations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                 signal[REG_MEAS_NUM_SIGNALS];           // Array of measurement with different filtering</t>
+  </si>
+  <si>
+    <t>struct reg_meas_rate                                              // Measurement rate estimate structure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    uint32_t              iter_counter;                           // Iteration counter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    uint32_t              history_index;                          // Index of most recent sample in history buffer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                 history_buf[REG_MEAS_RATE_BUF_MASK+1];  // History buffer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                 estimate;                               // Estimated rate using linear regression through 4 samples</t>
+  </si>
+  <si>
+    <t>struct reg_noise_and_tone                                         // Noise and tone generator structure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    uint32_t              iter_counter;                           // Iteration counter for simulated tone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    uint32_t              tone_half_period_iters;                 // Tone half period in iterations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    uint32_t              tone_toggle;                            // Tone toggle (0,1,0,1,...)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                 tone_amp;                               // Tone amplitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                 noise_pp;                               // Simulated measurement peak-peak noise level</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">void     regMeasFilterInit         (struct reg_meas_filter *filter, uint32_t </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>fir_length[2],</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">void     regMeasSetNoiseAndTone    (struct reg_noise_and_tone *noise_and_tone, float </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>noise_pp,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                    float </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>tone_amp,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t xml:space="preserve"> uint32_t </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>tone_half_period_iters);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                    uint32_t </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>extrapolation_len_iters,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t xml:space="preserve"> float </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>pos,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t xml:space="preserve"> float </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>neg,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t xml:space="preserve"> float </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>meas_delay_iters);</t>
+    </r>
+  </si>
+  <si>
+    <t>float    regLoadCurrentToFieldRT  (struct reg_load_pars *load, float i_meas);</t>
+  </si>
+  <si>
+    <t>float    regLoadFieldToCurrentRT  (struct reg_load_pars *load, float b_meas);</t>
+  </si>
+  <si>
+    <t>float    regLoadVrefSatRT         (struct reg_load_pars *load, float i_meas, float v_ref);</t>
+  </si>
+  <si>
+    <t>float    regLoadInverseVrefSatRT  (struct reg_load_pars *load, float i_meas, float v_ref_sat);</t>
+  </si>
+  <si>
+    <t>float    regLoadSatFactorRT       (struct reg_load_pars *load, float i_meas);</t>
+  </si>
+  <si>
+    <t>struct reg_load_pars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       ohms_ser;                       // Load series resistance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       ohms_par;                       // Load parallel resistance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       ohms_mag;                       // Load magnet resistance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       henrys;                         // Load inductance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       inv_henrys;                     // 1.0 / henrys clipped to 1.0E+20 to avoid infinities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       gauss_per_amp;                  // Field to current ratio for the magnet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       ohms;                           // Resistance corresponding to load pole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       tc;                             // Time constant for load pole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       gain0;                          // Load gain 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       gain1;                          // Load gain 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       ohms1;                          // Load gain 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       gain2;                          // Load gain 3 (steady state gain)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       ohms2;                          // Load gain 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       gain10;                         // Load gain 1/Load gain 0 : Rp insignificance factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                // if gain10 &gt; ~10 then Rp is insignificant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    struct reg_load_sat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        float                   henrys;                         // Inductance for i &gt; i_sat_end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        float                   i_start;                        // Current measurement at start of saturation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        float                   i_end;                          // Current measurement at end of saturation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        float                   i_delta;                        // i_sat_end - i_sat_start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        float                   b_end;                          // Field at i_sat_end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        float                   b_factor;                       // Parabolic factor for i_sat_start &lt; i &lt; i_sat_end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        float                   l_rate;                         // Inductance droop rate factor (/A)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        float                   l_clip;                         // Clip limit for saturation factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    } sat;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">void     regLoadInit              (struct reg_load_pars *load, float </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>ohms_ser,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t xml:space="preserve"> float </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>ohms_par,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t xml:space="preserve"> float </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>ohms_mag,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                   float </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>henrys,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t xml:space="preserve"> float </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>gauss_per_amp);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">void     regLoadInitSat           (struct reg_load_pars *load, float </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>henrys_sat,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t xml:space="preserve"> float </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>i_sat_start,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t xml:space="preserve"> float </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>i_sat_end);</t>
+    </r>
+  </si>
+  <si>
+    <t>void     regLimMeasRT           (struct reg_lim_meas *lim_meas, float meas);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                 uint32_t invert_limits);</t>
+  </si>
+  <si>
+    <t>void     regLimVrefCalcRT       (struct reg_lim_ref *lim_v_ref, float i_meas);</t>
+  </si>
+  <si>
+    <t>float    regLimRefRT            (struct reg_lim_ref *lim_ref, float period, float ref, float prev_ref);</t>
+  </si>
+  <si>
+    <t>struct reg_lim_meas                                             // Measurement limits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    uint32_t                    invert_limits;                  // Invert the limits before use flag (e.g. polarity switch is negative)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       pos_trip;                       // Positive measurement trip limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       neg_trip;                       // Negative measurement trip limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       low;                            // Low measurement threshold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       zero;                           // Zero measurement threshold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       rms2_trip;                      // Squared RMS trip threshold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       rms2_warning;                   // Squared RMS warning threshold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       rms2_warning_hysteresis;        // Squared RMS warning threshold with hysteresis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       meas2_filter;                   // Filtered square of the measurement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       meas2_filter_factor;            // First order filter factor for square of measurement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       low_hysteresis;                 // Low measurement threshold with hysteresis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       zero_hysteresis;                // Zero measurement threshold with hysteresis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    struct                                                      // Measurement limit flags</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        uint32_t                trip;                           // Measurement exceeds pos or neg trip limits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        uint32_t                rms_trip;                       // Filtered square of the measurement exceeds trip level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        uint32_t                rms_warning;                    // Filtered square of the measurement exceeds warning level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        uint32_t                low;                            // Absolute measurement is below low threshold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        uint32_t                zero;                           // Absolute measurement is below zero threshold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    } flags;</t>
+  </si>
+  <si>
+    <t>struct reg_lim_ref                                              // Reference limits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       max_clip;                       // Max ref clip limit from max_clip_user or Q41 limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       min_clip;                       // Min ref clip limit from min_clip_user or Q41 limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       rate_clip;                      // Abs ref rate clip limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       max_clip_user;                  // Maximum reference clip limit from user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       min_clip_user;                  // Minimum reference clip limit from user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       i_quadrants41_max;              // i_quadrants41[1] or -1.0E10 if no Q41 limits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       v0;                             // Voltage limit for i_meas = 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       dvdi;                           // Voltage limit slope with i_meas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    struct                                                      // Reference limit flags</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        uint32_t                unipolar;                       // Unipolar flag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        uint32_t                clip;                           // Ref is being clipped to [max_clip,min_clip] range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        uint32_t                rate;                           // Ref rate is being clipped to +/-rate_clip range</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">void     regLimMeasInit         (struct reg_lim_meas *lim_meas, float </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>pos_lim,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t xml:space="preserve"> float </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>neg_lim,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                 float </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>low_lim,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t xml:space="preserve"> float </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>zero_lim,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t xml:space="preserve"> uint32_t </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>invert_limits);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">void     regLimMeasRmsInit      (struct reg_lim_meas *lim_meas, float </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>rms_trip,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t xml:space="preserve"> float </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>rms_warning,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t xml:space="preserve"> float </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>rms_tc,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t xml:space="preserve"> float iter_period);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">void     regLimRefInit          (struct reg_lim_ref *lim_ref, float </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>pos_lim,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t xml:space="preserve"> float </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>neg_lim,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t xml:space="preserve"> float </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>rate_lim,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">void     regLimVrefInit         (struct reg_lim_ref *lim_v_ref, float </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>pos_lim,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t xml:space="preserve"> float </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>neg_lim,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t xml:space="preserve"> float </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>rate_lim,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                 float </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>i_quadrants41[2],</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t xml:space="preserve"> float </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>v_quadrants41[2],</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t xml:space="preserve"> uint32_t </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>invert_limits);</t>
     </r>
   </si>
 </sst>
@@ -931,10 +1743,1349 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C60"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="3.6640625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="149.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3">
+      <c r="C2" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3">
+      <c r="B3" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4" s="5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8" s="5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3">
+      <c r="B9" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3">
+      <c r="B10" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3">
+      <c r="B11" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="B12" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3">
+      <c r="C14" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3">
+      <c r="B15" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3">
+      <c r="B16" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" s="5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" s="5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" s="5" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2">
+      <c r="B26" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2">
+      <c r="B27" s="5" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28" s="5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2">
+      <c r="B30" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2">
+      <c r="B31" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2">
+      <c r="B32" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3">
+      <c r="B33" s="5" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3">
+      <c r="B34" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3">
+      <c r="B35" s="5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3">
+      <c r="B36" s="5" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3">
+      <c r="B37" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3">
+      <c r="B38" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3">
+      <c r="B40" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3">
+      <c r="B41" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3">
+      <c r="B42" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3">
+      <c r="B43" s="5" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3">
+      <c r="B44" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3">
+      <c r="B45" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3">
+      <c r="B47" s="5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3">
+      <c r="B48" s="5" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2">
+      <c r="B50" s="5" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2">
+      <c r="B51" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2">
+      <c r="B52" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2">
+      <c r="B54" s="5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2">
+      <c r="B55" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2">
+      <c r="B56" s="5" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2">
+      <c r="B57" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2">
+      <c r="B58" s="5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2">
+      <c r="B59" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2">
+      <c r="B60" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="3.6640625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="139.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7">
+      <c r="C2" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7">
+      <c r="B3" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7">
+      <c r="C12" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7">
+      <c r="B13" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7">
+      <c r="B14" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7">
+      <c r="B15" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7">
+      <c r="B16" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="B17" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="B18" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7">
+      <c r="B19" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="B20" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7">
+      <c r="B21" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7">
+      <c r="B22" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7">
+      <c r="B23" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7">
+      <c r="B24" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="B25" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7">
+      <c r="B26" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7">
+      <c r="B27" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7">
+      <c r="B28" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7">
+      <c r="B29" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7">
+      <c r="B30" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" s="2" customFormat="1">
+      <c r="B31" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+    </row>
+    <row r="32" spans="2:7" s="2" customFormat="1">
+      <c r="B32" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" spans="2:7" s="2" customFormat="1">
+      <c r="B33" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+    </row>
+    <row r="34" spans="2:7" s="2" customFormat="1">
+      <c r="B34" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+    </row>
+    <row r="35" spans="2:7" s="2" customFormat="1">
+      <c r="B35" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+    </row>
+    <row r="36" spans="2:7" s="2" customFormat="1">
+      <c r="B36" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+    </row>
+    <row r="37" spans="2:7" s="2" customFormat="1">
+      <c r="B37" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+    </row>
+    <row r="38" spans="2:7" s="2" customFormat="1">
+      <c r="B38" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+    </row>
+    <row r="39" spans="2:7" s="2" customFormat="1">
+      <c r="B39" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+    </row>
+    <row r="40" spans="2:7" s="2" customFormat="1">
+      <c r="B40" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+    </row>
+    <row r="41" spans="2:7" s="2" customFormat="1">
+      <c r="B41" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+    </row>
+    <row r="42" spans="2:7" s="2" customFormat="1">
+      <c r="B42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G59"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="3.6640625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="133.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7">
+      <c r="C2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="2:7">
+      <c r="B3" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7">
+      <c r="B11" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7">
+      <c r="C13" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7">
+      <c r="B14" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7">
+      <c r="B15" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7">
+      <c r="B16" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="B17" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="B18" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="B20" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7">
+      <c r="B21" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7">
+      <c r="B22" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7">
+      <c r="B24" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="B25" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7">
+      <c r="B27" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7">
+      <c r="B28" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7">
+      <c r="B29" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7">
+      <c r="B31" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" s="2" customFormat="1">
+      <c r="B32" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" spans="2:7" s="2" customFormat="1">
+      <c r="B33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+    </row>
+    <row r="34" spans="2:7" s="2" customFormat="1">
+      <c r="B34" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+    </row>
+    <row r="35" spans="2:7" s="2" customFormat="1">
+      <c r="B35" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+    </row>
+    <row r="36" spans="2:7" s="2" customFormat="1">
+      <c r="B36" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+    </row>
+    <row r="37" spans="2:7" s="2" customFormat="1">
+      <c r="B37" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+    </row>
+    <row r="38" spans="2:7" s="2" customFormat="1">
+      <c r="B38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+    </row>
+    <row r="39" spans="2:7" s="2" customFormat="1">
+      <c r="B39" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+    </row>
+    <row r="40" spans="2:7" s="2" customFormat="1">
+      <c r="B40" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+    </row>
+    <row r="41" spans="2:7" s="2" customFormat="1">
+      <c r="B41" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+    </row>
+    <row r="42" spans="2:7" s="2" customFormat="1">
+      <c r="B42" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+    </row>
+    <row r="43" spans="2:7" s="2" customFormat="1">
+      <c r="B43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+    </row>
+    <row r="44" spans="2:7" s="2" customFormat="1">
+      <c r="B44" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+    </row>
+    <row r="45" spans="2:7" s="2" customFormat="1">
+      <c r="B45" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+    </row>
+    <row r="46" spans="2:7" s="2" customFormat="1">
+      <c r="B46" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+    </row>
+    <row r="47" spans="2:7">
+      <c r="B47" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7">
+      <c r="B48" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4">
+      <c r="B49" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4">
+      <c r="B50" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4">
+      <c r="B52" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4">
+      <c r="B53" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4">
+      <c r="B54" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4">
+      <c r="B55" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4">
+      <c r="B56" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4">
+      <c r="B57" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4">
+      <c r="B58" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4">
+      <c r="B59" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G57"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="3.6640625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="133.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7">
+      <c r="C2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="2:7">
+      <c r="B3" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7">
+      <c r="B11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7">
+      <c r="B12" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7">
+      <c r="C14" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7">
+      <c r="B15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7">
+      <c r="B16" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3">
+      <c r="B20" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3">
+      <c r="B23" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3">
+      <c r="B24" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3">
+      <c r="B25" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3">
+      <c r="B26" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3">
+      <c r="B27" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3">
+      <c r="B28" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3">
+      <c r="B29" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3">
+      <c r="B30" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3">
+      <c r="B31" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3">
+      <c r="B32" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2">
+      <c r="B38" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2">
+      <c r="B39" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2">
+      <c r="B41" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2">
+      <c r="B42" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2">
+      <c r="B43" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2">
+      <c r="B44" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2">
+      <c r="B45" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2">
+      <c r="B46" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2">
+      <c r="B47" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4">
+      <c r="B49" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4">
+      <c r="B50" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4">
+      <c r="B51" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4">
+      <c r="B52" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4">
+      <c r="B53" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4">
+      <c r="B54" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4">
+      <c r="B55" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4">
+      <c r="B56" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4">
+      <c r="B57" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1240,341 +3391,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G57"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="3.6640625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="133.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="5"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:7">
-      <c r="C2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="2:7">
-      <c r="B3" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7">
-      <c r="B4" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7">
-      <c r="B5" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7">
-      <c r="B6" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7">
-      <c r="B7" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7">
-      <c r="B8" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7">
-      <c r="B9" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7">
-      <c r="B10" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7">
-      <c r="B11" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7">
-      <c r="B12" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7">
-      <c r="C14" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7">
-      <c r="B15" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7">
-      <c r="B16" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3">
-      <c r="B17" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3">
-      <c r="B18" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3">
-      <c r="B19" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3">
-      <c r="B20" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3">
-      <c r="B22" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3">
-      <c r="B23" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3">
-      <c r="B24" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3">
-      <c r="B25" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3">
-      <c r="B26" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3">
-      <c r="B27" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3">
-      <c r="B28" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3">
-      <c r="B29" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3">
-      <c r="B30" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3">
-      <c r="B31" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3">
-      <c r="B32" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2">
-      <c r="B33" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2">
-      <c r="B34" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2">
-      <c r="B35" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2">
-      <c r="B36" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2">
-      <c r="B37" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2">
-      <c r="B38" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="39" spans="2:2">
-      <c r="B39" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="40" spans="2:2">
-      <c r="B40" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="41" spans="2:2">
-      <c r="B41" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="42" spans="2:2">
-      <c r="B42" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="43" spans="2:2">
-      <c r="B43" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="44" spans="2:2">
-      <c r="B44" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="45" spans="2:2">
-      <c r="B45" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="46" spans="2:2">
-      <c r="B46" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="47" spans="2:2">
-      <c r="B47" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4">
-      <c r="B49" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4">
-      <c r="B50" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4">
-      <c r="B51" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4">
-      <c r="B52" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4">
-      <c r="B53" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4">
-      <c r="B54" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4">
-      <c r="B55" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="56" spans="2:4">
-      <c r="B56" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4">
-      <c r="B57" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update libcc/resources/libreg.xlsx to complete analysis of all structures in libreg
</commit_message>
<xml_diff>
--- a/libcc/resources/libreg.xlsx
+++ b/libcc/resources/libreg.xlsx
@@ -4,14 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16620" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16620" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="lim.h" sheetId="6" r:id="rId1"/>
-    <sheet name="load.h" sheetId="5" r:id="rId2"/>
-    <sheet name="meas.h" sheetId="4" r:id="rId3"/>
-    <sheet name="rst.h" sheetId="2" r:id="rId4"/>
-    <sheet name="sim.h" sheetId="1" r:id="rId5"/>
+    <sheet name="conv.h" sheetId="9" r:id="rId1"/>
+    <sheet name="err.h" sheetId="8" r:id="rId2"/>
+    <sheet name="delay.h" sheetId="7" r:id="rId3"/>
+    <sheet name="lim.h" sheetId="6" r:id="rId4"/>
+    <sheet name="load.h" sheetId="5" r:id="rId5"/>
+    <sheet name="meas.h" sheetId="4" r:id="rId6"/>
+    <sheet name="rst.h" sheetId="2" r:id="rId7"/>
+    <sheet name="sim.h" sheetId="1" r:id="rId8"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="230">
   <si>
     <t>void     regSimLoadTcError      (struct reg_sim_load_pars *sim_load_pars, struct reg_load_pars *load_pars, float sim_load_tc_error);</t>
   </si>
@@ -1272,6 +1275,77 @@
       </rPr>
       <t>invert_limits);</t>
     </r>
+  </si>
+  <si>
+    <t>void     regErrResetLimitsVarsRT  (struct reg_err *err);</t>
+  </si>
+  <si>
+    <t>void     regErrCheckLimitsRT      (struct reg_err *err, uint32_t enable_err, uint32_t enable_max_abs_err,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                   float delayed_ref, float meas);</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">void     regErrInitLimits         (struct reg_err *err, float </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>warning_threshold,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t xml:space="preserve"> float </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>fault_threshold);</t>
+    </r>
+  </si>
+  <si>
+    <t>struct reg_err_limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       threshold;                      // Limit threshold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       filter;                         // Threshold exceeded flag filter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    uint32_t                    flag;                           // Limit exceeded flag</t>
+  </si>
+  <si>
+    <t>struct reg_err</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       delayed_ref;                    // Delayed reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       err;                            // Regulation error = delayed_ref - meas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    float                       max_abs_err;                    // Max absolute error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    struct reg_err_limit        warning;                        // Warning limit structure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    struct reg_err_limit        fault;                          // Fault limit structure</t>
+  </si>
+  <si>
+    <t>Thresholds can be changed</t>
   </si>
 </sst>
 </file>
@@ -1743,9 +1817,827 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G57"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="3.6640625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="133.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7">
+      <c r="C2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="2:7">
+      <c r="B3" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7">
+      <c r="B11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7">
+      <c r="B12" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7">
+      <c r="C14" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7">
+      <c r="B15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7">
+      <c r="B16" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3">
+      <c r="B20" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3">
+      <c r="B23" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3">
+      <c r="B24" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3">
+      <c r="B25" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3">
+      <c r="B26" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3">
+      <c r="B27" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3">
+      <c r="B28" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3">
+      <c r="B29" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3">
+      <c r="B30" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3">
+      <c r="B31" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3">
+      <c r="B32" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2">
+      <c r="B38" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2">
+      <c r="B39" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2">
+      <c r="B41" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2">
+      <c r="B42" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2">
+      <c r="B43" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2">
+      <c r="B44" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2">
+      <c r="B45" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2">
+      <c r="B46" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2">
+      <c r="B47" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4">
+      <c r="B49" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4">
+      <c r="B50" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4">
+      <c r="B51" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4">
+      <c r="B52" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4">
+      <c r="B53" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4">
+      <c r="B54" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4">
+      <c r="B55" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4">
+      <c r="B56" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4">
+      <c r="B57" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="3.6640625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="133.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3">
+      <c r="C2" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3">
+      <c r="B3" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6" s="5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="C8" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3">
+      <c r="B9" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3">
+      <c r="B10" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3">
+      <c r="B11" s="5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="B12" s="5" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="B13" s="5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3">
+      <c r="B14" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="5" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21" s="5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="B22" s="5" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="B23" s="5" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G57"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="3.6640625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="133.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7">
+      <c r="C2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="2:7">
+      <c r="B3" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7">
+      <c r="B11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7">
+      <c r="B12" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7">
+      <c r="C14" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7">
+      <c r="B15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7">
+      <c r="B16" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3">
+      <c r="B20" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3">
+      <c r="B23" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3">
+      <c r="B24" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3">
+      <c r="B25" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3">
+      <c r="B26" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3">
+      <c r="B27" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3">
+      <c r="B28" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3">
+      <c r="B29" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3">
+      <c r="B30" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3">
+      <c r="B31" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3">
+      <c r="B32" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2">
+      <c r="B38" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2">
+      <c r="B39" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2">
+      <c r="B41" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2">
+      <c r="B42" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2">
+      <c r="B43" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2">
+      <c r="B44" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2">
+      <c r="B45" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2">
+      <c r="B46" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2">
+      <c r="B47" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4">
+      <c r="B49" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4">
+      <c r="B50" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4">
+      <c r="B51" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4">
+      <c r="B52" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4">
+      <c r="B53" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4">
+      <c r="B54" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4">
+      <c r="B55" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4">
+      <c r="B56" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4">
+      <c r="B57" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -2059,7 +2951,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G42"/>
   <sheetViews>
@@ -2358,7 +3250,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G59"/>
   <sheetViews>
@@ -2743,7 +3635,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G57"/>
   <sheetViews>
@@ -3080,7 +3972,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F48"/>
   <sheetViews>

</xml_diff>